<commit_message>
documentation, lifeform and user factories, password encryption
</commit_message>
<xml_diff>
--- a/Documentation/Gantt-projektplanlægger.xlsx
+++ b/Documentation/Gantt-projektplanlægger.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D459E57F-773F-493C-A7E6-60596DE1EA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEDA5A4-11D1-4C4A-881D-F81CBB7733F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplanlægger" sheetId="1" r:id="rId1"/>
@@ -616,6 +616,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -624,33 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1063,8 +1063,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1101,66 +1101,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="29" t="s">
+      <c r="W2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="36"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AH2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="27" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1187,7 +1187,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -1459,7 +1459,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D9" s="7">
         <v>2</v>
@@ -1482,7 +1482,8 @@
         <v>1</v>
       </c>
       <c r="D10" s="7">
-        <v>30</v>
+        <f>19+4</f>
+        <v>23</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
@@ -1491,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="8">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1502,7 +1503,8 @@
         <v>6</v>
       </c>
       <c r="D11" s="7">
-        <v>25</v>
+        <f>12+4</f>
+        <v>16</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -1519,10 +1521,11 @@
         <v>24</v>
       </c>
       <c r="C12" s="7">
-        <v>0</v>
+        <f>4+4</f>
+        <v>8</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -1542,16 +1545,16 @@
         <v>3</v>
       </c>
       <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
         <v>3</v>
       </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
       <c r="F13" s="7">
         <v>0</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1579,10 +1582,10 @@
         <v>27</v>
       </c>
       <c r="C15" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D15" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="7">
         <v>0</v>
@@ -1599,10 +1602,10 @@
         <v>28</v>
       </c>
       <c r="C16" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="7">
         <v>0</v>
@@ -1619,10 +1622,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="7">
         <v>0</v>
@@ -1631,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1639,19 +1642,19 @@
         <v>30</v>
       </c>
       <c r="C18" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F18" s="7">
         <v>0</v>
       </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1659,19 +1662,19 @@
         <v>31</v>
       </c>
       <c r="C19" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1679,19 +1682,19 @@
         <v>32</v>
       </c>
       <c r="C20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1699,10 +1702,10 @@
         <v>33</v>
       </c>
       <c r="C21" s="7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D21" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E21" s="7">
         <v>0</v>
@@ -1719,19 +1722,19 @@
         <v>34</v>
       </c>
       <c r="C22" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D22" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
       </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1739,19 +1742,19 @@
         <v>35</v>
       </c>
       <c r="C23" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F23" s="7">
         <v>0</v>
       </c>
       <c r="G23" s="8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1759,10 +1762,10 @@
         <v>36</v>
       </c>
       <c r="C24" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D24" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -1779,10 +1782,10 @@
         <v>37</v>
       </c>
       <c r="C25" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D25" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
@@ -1799,10 +1802,10 @@
         <v>38</v>
       </c>
       <c r="C26" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D26" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
@@ -1819,19 +1822,19 @@
         <v>39</v>
       </c>
       <c r="C27" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D27" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F27" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1896,17 +1899,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
implemented deletion of message
</commit_message>
<xml_diff>
--- a/Documentation/Gantt-projektplanlægger.xlsx
+++ b/Documentation/Gantt-projektplanlægger.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEDA5A4-11D1-4C4A-881D-F81CBB7733F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561A4F47-6F8E-4E20-90C7-9ADE9D19F80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>AKTIVITET</t>
   </si>
   <si>
-    <t>Aktivitet 24</t>
-  </si>
-  <si>
     <t>Aktivitet 25</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Processerrapport</t>
   </si>
   <si>
-    <t>App</t>
-  </si>
-  <si>
     <t>Kravspecifikationer</t>
   </si>
   <si>
@@ -236,14 +230,20 @@
     <t>Context</t>
   </si>
   <si>
-    <t>Backend base implementering</t>
+    <t>Backend  implementering</t>
+  </si>
+  <si>
+    <t>App implementering</t>
+  </si>
+  <si>
+    <t>App/SignalR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -345,13 +345,6 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1" tint="0.24994659260841701"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -540,7 +533,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,8 +606,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
@@ -625,9 +627,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -642,15 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1063,14 +1053,14 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.125" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.75" style="4" customWidth="1"/>
     <col min="8" max="27" width="3.25" style="1"/>
@@ -1095,76 +1085,76 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="29" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="25" t="s">
+      <c r="X2" s="29"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="25" t="s">
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="26"/>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="26"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="F3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>11</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>12</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
@@ -1187,12 +1177,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1376,7 +1366,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1396,27 +1386,27 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="7">
         <v>2</v>
       </c>
       <c r="E6" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G6" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1431,32 +1421,32 @@
         <v>3</v>
       </c>
       <c r="G7" s="8">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" s="7">
         <v>4</v>
       </c>
       <c r="E8" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1476,7 +1466,7 @@
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
@@ -1497,28 +1487,27 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7">
         <v>6</v>
       </c>
       <c r="D11" s="7">
-        <f>12+4</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
       </c>
       <c r="G11" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
-        <v>24</v>
+      <c r="B12" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="7">
         <f>4+4</f>
@@ -1539,7 +1528,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
         <v>3</v>
@@ -1551,21 +1540,21 @@
         <v>3</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="8">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="7">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D14" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -1579,47 +1568,47 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D15" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E15" s="7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="7">
         <v>3</v>
@@ -1628,18 +1617,18 @@
         <v>2</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="8">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="7">
         <v>4</v>
@@ -1651,15 +1640,15 @@
         <v>4</v>
       </c>
       <c r="F18" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" s="8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="7">
         <v>3</v>
@@ -1679,7 +1668,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
@@ -1699,10 +1688,10 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="7">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D21" s="7">
         <v>4</v>
@@ -1719,7 +1708,7 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="7">
         <v>4</v>
@@ -1734,12 +1723,12 @@
         <v>0</v>
       </c>
       <c r="G22" s="8">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="7">
         <v>4</v>
@@ -1748,18 +1737,18 @@
         <v>2</v>
       </c>
       <c r="E23" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G23" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="7">
         <v>8</v>
@@ -1768,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F24" s="7">
         <v>0</v>
@@ -1779,7 +1768,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="7">
         <v>8</v>
@@ -1788,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F25" s="7">
         <v>0</v>
@@ -1799,7 +1788,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="7">
         <v>8</v>
@@ -1808,7 +1797,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F26" s="7">
         <v>0</v>
@@ -1819,19 +1808,19 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C27" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G27" s="8">
         <v>1</v>
@@ -1839,13 +1828,13 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C28" s="7">
         <v>0</v>
       </c>
       <c r="D28" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" s="7">
         <v>0</v>
@@ -1859,7 +1848,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" s="7">
         <v>0</v>
@@ -1879,7 +1868,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="7">
         <v>0</v>
@@ -1899,17 +1888,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
working on displaying details
</commit_message>
<xml_diff>
--- a/Documentation/Gantt-projektplanlægger.xlsx
+++ b/Documentation/Gantt-projektplanlægger.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561A4F47-6F8E-4E20-90C7-9ADE9D19F80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618B21C1-86D9-43F8-9174-439483293338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,6 +606,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -614,33 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1053,8 +1053,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1088,69 +1088,69 @@
         <v>9</v>
       </c>
       <c r="H2" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="33"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="30"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="35"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="32"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="28" t="s">
+      <c r="AA2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="29"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1177,7 +1177,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -1517,13 +1517,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1757,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F24" s="7">
         <v>0</v>
@@ -1777,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F25" s="7">
         <v>0</v>
@@ -1797,7 +1797,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F26" s="7">
         <v>0</v>
@@ -1888,17 +1888,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
working on tests and updated Gantt
</commit_message>
<xml_diff>
--- a/Documentation/Gantt-projektplanlægger.xlsx
+++ b/Documentation/Gantt-projektplanlægger.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618B21C1-86D9-43F8-9174-439483293338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C10C86-BC5E-4769-8B8C-889CE39A2CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,6 +606,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -615,9 +627,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -632,15 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1053,8 +1053,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1088,69 +1088,69 @@
         <v>9</v>
       </c>
       <c r="H2" s="15">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="30"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="32"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="24" t="s">
+      <c r="AH2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1177,7 +1177,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -1580,10 +1580,10 @@
         <v>8</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G15" s="8">
-        <v>0.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="8">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1888,17 +1888,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
added more things for documentation and report
</commit_message>
<xml_diff>
--- a/Documentation/Gantt-projektplanlægger.xlsx
+++ b/Documentation/Gantt-projektplanlægger.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEABE23-3752-41E6-9BBF-E7C8704C00DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E661F96-E9B8-4C3D-A64E-E95B1F9832A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplanlægger" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Projektplanlægger</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>AKTIVITET</t>
-  </si>
-  <si>
-    <t>Aktivitet 25</t>
-  </si>
-  <si>
-    <t>Aktivitet 26</t>
   </si>
   <si>
     <t>STARTDATO FOR PLAN</t>
@@ -1051,10 +1045,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO29"/>
+  <dimension ref="B1:BO27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1085,14 +1079,14 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2" s="15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
@@ -1100,7 +1094,7 @@
       <c r="O2" s="30"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R2" s="31"/>
       <c r="S2" s="31"/>
@@ -1108,13 +1102,13 @@
       <c r="U2" s="30"/>
       <c r="V2" s="18"/>
       <c r="W2" s="24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="X2" s="25"/>
       <c r="Y2" s="32"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AB2" s="25"/>
       <c r="AC2" s="25"/>
@@ -1123,7 +1117,7 @@
       <c r="AF2" s="25"/>
       <c r="AG2" s="20"/>
       <c r="AH2" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AI2" s="25"/>
       <c r="AJ2" s="25"/>
@@ -1139,22 +1133,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="F3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="35" t="s">
+      <c r="G3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>10</v>
-      </c>
       <c r="H3" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="11"/>
@@ -1366,7 +1360,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1384,12 +1378,12 @@
         <v>1</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7">
         <v>2</v>
@@ -1407,12 +1401,12 @@
         <v>1</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1430,12 +1424,12 @@
         <v>1</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="7">
         <v>4</v>
@@ -1453,12 +1447,12 @@
         <v>1</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1476,12 +1470,12 @@
         <v>0</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
@@ -1500,12 +1494,12 @@
         <v>0.7</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>6</v>
@@ -1523,12 +1517,12 @@
         <v>0.7</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
         <v>3</v>
@@ -1546,12 +1540,12 @@
         <v>1</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="7">
         <v>14</v>
@@ -1569,12 +1563,12 @@
         <v>1</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="9">
         <v>10</v>
@@ -1592,12 +1586,12 @@
         <v>1</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="7">
         <v>3</v>
@@ -1615,12 +1609,12 @@
         <v>1</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="7">
         <v>3</v>
@@ -1638,12 +1632,12 @@
         <v>1</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="7">
         <v>4</v>
@@ -1661,12 +1655,12 @@
         <v>1</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="7">
         <v>3</v>
@@ -1684,12 +1678,12 @@
         <v>1</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
@@ -1707,12 +1701,12 @@
         <v>1</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7">
         <v>14</v>
@@ -1730,12 +1724,12 @@
         <v>0</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="7">
         <v>4</v>
@@ -1753,12 +1747,12 @@
         <v>1</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="7">
         <v>4</v>
@@ -1776,12 +1770,12 @@
         <v>1</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="7">
         <v>8</v>
@@ -1799,12 +1793,12 @@
         <v>1</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="7">
         <v>8</v>
@@ -1822,12 +1816,12 @@
         <v>1</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" s="7">
         <v>8</v>
@@ -1845,12 +1839,12 @@
         <v>1</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="7">
         <v>2</v>
@@ -1868,12 +1862,12 @@
         <v>1</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C27" s="7">
         <v>0</v>
@@ -1891,53 +1885,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7">
-        <v>0</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
-        <v>0</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +1902,7 @@
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO29">
+  <conditionalFormatting sqref="H5:BO27">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>ProcentdelFuldført</formula>
     </cfRule>
@@ -1980,7 +1928,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:BO30">
+  <conditionalFormatting sqref="B28:BO28">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
made it possible to post a message on the hub, added text file that explains how to do from postman
</commit_message>
<xml_diff>
--- a/Documentation/Gantt-projektplanlægger.xlsx
+++ b/Documentation/Gantt-projektplanlægger.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E661F96-E9B8-4C3D-A64E-E95B1F9832A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637B1800-9E96-4965-8970-3A645C08137C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplanlægger" sheetId="1" r:id="rId1"/>
@@ -600,6 +600,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -609,9 +621,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -626,15 +635,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1048,7 +1048,7 @@
   <dimension ref="B1:BO27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1082,69 +1082,69 @@
         <v>7</v>
       </c>
       <c r="H2" s="15">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="30"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="28" t="s">
+      <c r="Q2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="30"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="33"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="32"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="24" t="s">
+      <c r="AH2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="30" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1171,7 +1171,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
@@ -1461,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -1890,17 +1890,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO27">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>